<commit_message>
Corrección en diccionario de datos
</commit_message>
<xml_diff>
--- a/Base de datos/DicDatos.xlsx
+++ b/Base de datos/DicDatos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico&amp;Sebas\Desktop\Trabajos\Bases2\proyecto_final\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Estudio\BD2\Proyecto\proyecto_final\Base de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="93">
   <si>
     <t>Atributo</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Empresa o universidad</t>
   </si>
   <si>
-    <t>Calificación de la institución dentro de la plataforma</t>
-  </si>
-  <si>
     <t>id_estudiante</t>
   </si>
   <si>
@@ -140,21 +137,9 @@
     <t>date</t>
   </si>
   <si>
-    <t>Nombre estudiante</t>
-  </si>
-  <si>
-    <t>Apellido estudiante</t>
-  </si>
-  <si>
-    <t>Usuario de ingreso estudiante</t>
-  </si>
-  <si>
     <t>Fecha de nacimiento del estudiante</t>
   </si>
   <si>
-    <t>nacionalidad estudiante</t>
-  </si>
-  <si>
     <t>Identificador del plan adquirido por el estutudiante</t>
   </si>
   <si>
@@ -257,9 +242,6 @@
     <t>estado</t>
   </si>
   <si>
-    <t>Estado actual del estudiante dentro de la especialización</t>
-  </si>
-  <si>
     <t>ESTUDIANTE_CURSO</t>
   </si>
   <si>
@@ -290,7 +272,37 @@
     <t>CURSO_PLAN</t>
   </si>
   <si>
-    <t>Estado actual del estudiante en el curso</t>
+    <t>Nombre de la institución</t>
+  </si>
+  <si>
+    <t>Calificación de la institución dentro de la plataforma, indica su reputación.</t>
+  </si>
+  <si>
+    <t>Nombre del estudiante</t>
+  </si>
+  <si>
+    <t>Apellido del estudiante</t>
+  </si>
+  <si>
+    <t>Usuario de ingreso del estudiante</t>
+  </si>
+  <si>
+    <t>nacionalidad del estudiante</t>
+  </si>
+  <si>
+    <t>Nombre del curso</t>
+  </si>
+  <si>
+    <t>Nombre de la especialización</t>
+  </si>
+  <si>
+    <t>Id de la institución que ofrece la especialización</t>
+  </si>
+  <si>
+    <t>Estado de la especialización para el estudiante. EJ: 'En curso'</t>
+  </si>
+  <si>
+    <t>Estado actual del curso para el estudiante. Ej:'En curso'</t>
   </si>
 </sst>
 </file>
@@ -4294,8 +4306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4303,7 +4315,7 @@
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
     <col min="6" max="7" width="10.140625" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
@@ -4352,7 +4364,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
@@ -4464,7 +4476,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
@@ -4559,10 +4571,10 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
@@ -4592,7 +4604,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>12</v>
@@ -4661,14 +4673,14 @@
     </row>
     <row r="20" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="11" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>12</v>
@@ -4685,7 +4697,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -4723,10 +4735,10 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
@@ -4756,7 +4768,7 @@
         <v>30</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>12</v>
@@ -4773,7 +4785,7 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>25</v>
@@ -4782,7 +4794,7 @@
         <v>30</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>12</v>
@@ -4799,7 +4811,7 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>25</v>
@@ -4808,7 +4820,7 @@
         <v>30</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>12</v>
@@ -4825,14 +4837,14 @@
     </row>
     <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>12</v>
@@ -4849,7 +4861,7 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>25</v>
@@ -4858,7 +4870,7 @@
         <v>20</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>12</v>
@@ -4878,11 +4890,11 @@
         <v>9</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>12</v>
@@ -4891,7 +4903,7 @@
         <v>11</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>11</v>
@@ -4899,7 +4911,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -4937,10 +4949,10 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
@@ -4970,7 +4982,7 @@
         <v>100</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>12</v>
@@ -4985,25 +4997,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>11</v>
@@ -5011,14 +5023,14 @@
     </row>
     <row r="37" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>12</v>
@@ -5035,14 +5047,14 @@
     </row>
     <row r="38" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>12</v>
@@ -5059,14 +5071,14 @@
     </row>
     <row r="39" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>12</v>
@@ -5093,7 +5105,7 @@
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
@@ -5131,10 +5143,10 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
@@ -5164,7 +5176,7 @@
         <v>100</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>12</v>
@@ -5184,20 +5196,20 @@
         <v>20</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="13" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>11</v>
@@ -5205,14 +5217,14 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>12</v>
@@ -5229,14 +5241,14 @@
     </row>
     <row r="47" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>12</v>
@@ -5253,7 +5265,7 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
@@ -5291,14 +5303,14 @@
     </row>
     <row r="51" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>11</v>
@@ -5307,7 +5319,7 @@
         <v>11</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>11</v>
@@ -5318,11 +5330,11 @@
         <v>9</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>11</v>
@@ -5331,7 +5343,7 @@
         <v>11</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I52" s="9" t="s">
         <v>11</v>
@@ -5349,7 +5361,7 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
@@ -5387,14 +5399,14 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>11</v>
@@ -5403,7 +5415,7 @@
         <v>11</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>11</v>
@@ -5411,14 +5423,14 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>11</v>
@@ -5427,7 +5439,7 @@
         <v>11</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I57" s="9" t="s">
         <v>11</v>
@@ -5435,7 +5447,7 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
@@ -5471,16 +5483,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>11</v>
@@ -5489,22 +5501,22 @@
         <v>11</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I61" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>11</v>
@@ -5513,7 +5525,7 @@
         <v>11</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I62" s="6" t="s">
         <v>11</v>
@@ -5521,7 +5533,7 @@
     </row>
     <row r="63" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>25</v>
@@ -5530,7 +5542,7 @@
         <v>50</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>12</v>
@@ -5547,7 +5559,7 @@
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
@@ -5585,14 +5597,14 @@
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>11</v>
@@ -5601,22 +5613,22 @@
         <v>11</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>11</v>
@@ -5625,15 +5637,15 @@
         <v>11</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>25</v>
@@ -5642,7 +5654,7 @@
         <v>50</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>12</v>
@@ -5657,16 +5669,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>12</v>
@@ -5681,16 +5693,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>12</v>
@@ -5705,16 +5717,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>12</v>
@@ -5731,7 +5743,7 @@
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
@@ -5769,14 +5781,14 @@
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>11</v>
@@ -5785,22 +5797,22 @@
         <v>11</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I76" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>11</v>
@@ -5809,7 +5821,7 @@
         <v>11</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>11</v>
@@ -5827,7 +5839,7 @@
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
@@ -5865,14 +5877,14 @@
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>11</v>
@@ -5881,7 +5893,7 @@
         <v>11</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I81" s="6" t="s">
         <v>11</v>
@@ -5892,11 +5904,11 @@
         <v>9</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>11</v>
@@ -5905,7 +5917,7 @@
         <v>11</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I82" s="9" t="s">
         <v>11</v>

</xml_diff>